<commit_message>
Netzplan Übung Lösung; Netzplan Übung2 für FIAE B
</commit_message>
<xml_diff>
--- a/Netzplan_Übung.xlsx
+++ b/Netzplan_Übung.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="30">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -296,7 +296,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -308,11 +308,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -320,7 +320,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -373,7 +373,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
     <dxf>
       <font>
         <b val="1"/>
@@ -389,6 +389,22 @@
     </dxf>
     <dxf>
       <font>
+        <b val="1"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+        <sz val="10"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
         <b val="1"/>
         <i val="0"/>
         <color rgb="FFFFFFFF"/>
@@ -514,13 +530,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>1080</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:rowOff>1800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>266400</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>7560</xdr:rowOff>
+      <xdr:rowOff>7920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -529,7 +545,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="812520" y="2601720"/>
+          <a:off x="812520" y="2602080"/>
           <a:ext cx="535680" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -554,15 +570,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1080</xdr:colOff>
+      <xdr:colOff>1440</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:rowOff>1800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>266760</xdr:colOff>
+      <xdr:colOff>267120</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>7560</xdr:rowOff>
+      <xdr:rowOff>7920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -571,7 +587,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="2164680" y="2601720"/>
+          <a:off x="2165040" y="2602080"/>
           <a:ext cx="536040" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -596,15 +612,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1080</xdr:colOff>
+      <xdr:colOff>1440</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>9360</xdr:rowOff>
+      <xdr:rowOff>9720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>266760</xdr:colOff>
+      <xdr:colOff>267120</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>15480</xdr:rowOff>
+      <xdr:rowOff>15840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -613,7 +629,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="2164680" y="3422520"/>
+          <a:off x="2165040" y="3422880"/>
           <a:ext cx="536040" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -640,13 +656,13 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>1080</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>9360</xdr:rowOff>
+      <xdr:rowOff>9720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>266400</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>15480</xdr:rowOff>
+      <xdr:rowOff>15840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -655,7 +671,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3517560" y="3422520"/>
+          <a:off x="3517560" y="3422880"/>
           <a:ext cx="535680" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -682,13 +698,13 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>1080</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:rowOff>1800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>266400</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>7560</xdr:rowOff>
+      <xdr:rowOff>7920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -697,7 +713,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3517560" y="2601720"/>
+          <a:off x="3517560" y="2602080"/>
           <a:ext cx="535680" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -724,13 +740,13 @@
       <xdr:col>18</xdr:col>
       <xdr:colOff>1080</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:rowOff>1800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>266400</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>7560</xdr:rowOff>
+      <xdr:rowOff>7920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -739,7 +755,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4870080" y="2601720"/>
+          <a:off x="4870080" y="2602080"/>
           <a:ext cx="535680" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -766,13 +782,13 @@
       <xdr:col>23</xdr:col>
       <xdr:colOff>720</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:rowOff>1800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>266400</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>7560</xdr:rowOff>
+      <xdr:rowOff>7920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -781,7 +797,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="6222240" y="2601720"/>
+          <a:off x="6222240" y="2602080"/>
           <a:ext cx="536400" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -808,13 +824,13 @@
       <xdr:col>18</xdr:col>
       <xdr:colOff>1080</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>9360</xdr:rowOff>
+      <xdr:rowOff>9720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>266400</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>15480</xdr:rowOff>
+      <xdr:rowOff>15840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -823,7 +839,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4870080" y="3422520"/>
+          <a:off x="4870080" y="3422880"/>
           <a:ext cx="535680" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -850,13 +866,13 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>1080</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>9360</xdr:rowOff>
+      <xdr:rowOff>9720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>266400</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>15480</xdr:rowOff>
+      <xdr:rowOff>15840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -865,7 +881,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3517560" y="4235400"/>
+          <a:off x="3517560" y="4235760"/>
           <a:ext cx="535680" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -890,13 +906,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1440</xdr:colOff>
+      <xdr:colOff>1800</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>8280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>253800</xdr:colOff>
+      <xdr:colOff>254160</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>8280</xdr:rowOff>
     </xdr:to>
@@ -907,7 +923,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="1082880" y="3421800"/>
+          <a:off x="1083240" y="3421800"/>
           <a:ext cx="252360" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -932,13 +948,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>1080</xdr:colOff>
+      <xdr:colOff>1440</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>8280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>253440</xdr:colOff>
+      <xdr:colOff>253800</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>8280</xdr:rowOff>
     </xdr:to>
@@ -949,7 +965,91 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="6222240" y="3421800"/>
+          <a:off x="6222600" y="3421800"/>
+          <a:ext cx="252360" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1800</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>8280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>254160</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>8280</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2435760" y="4234680"/>
+          <a:ext cx="252360" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>1800</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>8280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>254160</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>8280</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4870440" y="4234680"/>
           <a:ext cx="252360" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -975,98 +1075,14 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1440</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>8280</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>33480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>253800</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>8280</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="2435400" y="4234680"/>
-          <a:ext cx="252360" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="36000">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>1440</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>8280</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>253800</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>8280</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="4870080" y="4234680"/>
-          <a:ext cx="252360" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="36000">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1080</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>33120</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>9360</xdr:colOff>
+      <xdr:colOff>9720</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>163080</xdr:rowOff>
+      <xdr:rowOff>163440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1075,7 +1091,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2435040" y="3446280"/>
+          <a:off x="2435400" y="3446640"/>
           <a:ext cx="8280" cy="780120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1100,13 +1116,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>8640</xdr:colOff>
+      <xdr:colOff>9000</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>24120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>9000</xdr:colOff>
+      <xdr:colOff>9360</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>162360</xdr:rowOff>
     </xdr:to>
@@ -1117,7 +1133,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5147640" y="3437640"/>
+          <a:off x="5148000" y="3437640"/>
           <a:ext cx="360" cy="788400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1144,13 +1160,13 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:rowOff>1800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>154800</xdr:rowOff>
+      <xdr:rowOff>155160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1159,7 +1175,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1082160" y="2601720"/>
+          <a:off x="1082160" y="2602080"/>
           <a:ext cx="0" cy="803880"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1186,13 +1202,13 @@
       <xdr:col>24</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:rowOff>1800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>154800</xdr:rowOff>
+      <xdr:rowOff>155160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1201,7 +1217,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6492600" y="2601720"/>
+          <a:off x="6492600" y="2602080"/>
           <a:ext cx="0" cy="803880"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1226,6 +1242,893 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>258480</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>156600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>258480</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>156600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="799200" y="2594880"/>
+          <a:ext cx="541080" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>271080</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2164320" y="2601000"/>
+          <a:ext cx="541080" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>264600</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>271080</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1076040" y="3576240"/>
+          <a:ext cx="276840" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>258840</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>264960</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>163080</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1069920" y="2601000"/>
+          <a:ext cx="6120" cy="975240"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>720</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>6840</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2435040" y="4551480"/>
+          <a:ext cx="276840" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>271080</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2164320" y="3576240"/>
+          <a:ext cx="541080" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1080</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>7200</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>163080</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2435040" y="3576600"/>
+          <a:ext cx="6120" cy="975240"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>271080</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3516840" y="2600640"/>
+          <a:ext cx="541080" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>271080</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3516840" y="3576240"/>
+          <a:ext cx="541080" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>6840</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3516840" y="4551480"/>
+          <a:ext cx="276840" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1080</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>7200</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>163080</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3787560" y="3576600"/>
+          <a:ext cx="6120" cy="975240"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>720</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>271440</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4869720" y="2601000"/>
+          <a:ext cx="541080" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>720</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>271440</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4869720" y="3576240"/>
+          <a:ext cx="541080" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>720</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>6840</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5140080" y="4551480"/>
+          <a:ext cx="276840" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>91080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>6840</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>720</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5139720" y="2691360"/>
+          <a:ext cx="6480" cy="885240"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1080</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>7200</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>163080</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5140080" y="3576600"/>
+          <a:ext cx="6120" cy="975240"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>720</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>108720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>6840</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>108720</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5140080" y="2709360"/>
+          <a:ext cx="276840" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>720</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>271080</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6222240" y="2601000"/>
+          <a:ext cx="541080" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>720</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>6840</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6222240" y="3576240"/>
+          <a:ext cx="276840" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>720</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>6840</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="37" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6222240" y="4551480"/>
+          <a:ext cx="276840" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>264600</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>271080</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>162720</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6486120" y="2601360"/>
+          <a:ext cx="6480" cy="1950480"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -1233,11 +2136,11 @@
   </sheetPr>
   <dimension ref="A1:AB67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M8" activeCellId="0" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="3.83"/>
   </cols>
@@ -1489,22 +2392,55 @@
         <v>0</v>
       </c>
       <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="F15" s="6"/>
+      <c r="C15" s="8" t="n">
+        <f aca="false">A15+A17</f>
+        <v>2</v>
+      </c>
+      <c r="F15" s="6" t="n">
+        <f aca="false">C15</f>
+        <v>2</v>
+      </c>
       <c r="G15" s="7"/>
-      <c r="H15" s="8"/>
-      <c r="K15" s="6"/>
+      <c r="H15" s="8" t="n">
+        <f aca="false">F15+F17</f>
+        <v>10</v>
+      </c>
+      <c r="K15" s="6" t="n">
+        <f aca="false">H15</f>
+        <v>10</v>
+      </c>
       <c r="L15" s="7"/>
-      <c r="M15" s="8"/>
-      <c r="P15" s="6"/>
+      <c r="M15" s="8" t="n">
+        <f aca="false">K15+K17</f>
+        <v>16</v>
+      </c>
+      <c r="P15" s="6" t="n">
+        <f aca="false">M15</f>
+        <v>16</v>
+      </c>
       <c r="Q15" s="7"/>
-      <c r="R15" s="8"/>
-      <c r="U15" s="6"/>
+      <c r="R15" s="8" t="n">
+        <f aca="false">P15+P17</f>
+        <v>21</v>
+      </c>
+      <c r="U15" s="6" t="n">
+        <f aca="false">R15</f>
+        <v>21</v>
+      </c>
       <c r="V15" s="7"/>
-      <c r="W15" s="8"/>
-      <c r="Z15" s="6"/>
+      <c r="W15" s="8" t="n">
+        <f aca="false">U15+U17</f>
+        <v>29</v>
+      </c>
+      <c r="Z15" s="6" t="n">
+        <f aca="false">MAX(W15,W20)</f>
+        <v>29</v>
+      </c>
       <c r="AA15" s="7"/>
-      <c r="AB15" s="8"/>
+      <c r="AB15" s="8" t="n">
+        <f aca="false">Z15+Z17</f>
+        <v>33</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
@@ -1543,69 +2479,160 @@
         <f aca="false">H2</f>
         <v>2</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
+      <c r="B17" s="11" t="n">
+        <f aca="false">C18-C15</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="11" t="n">
+        <f aca="false">MIN(F15,F20)-C15</f>
+        <v>0</v>
+      </c>
       <c r="F17" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
+      <c r="G17" s="11" t="n">
+        <f aca="false">H18-H15</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="11" t="n">
+        <f aca="false">K15-H15</f>
+        <v>0</v>
+      </c>
       <c r="K17" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
+      <c r="L17" s="11" t="n">
+        <f aca="false">M18-M15</f>
+        <v>0</v>
+      </c>
+      <c r="M17" s="11" t="n">
+        <f aca="false">P15-M15</f>
+        <v>0</v>
+      </c>
       <c r="P17" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
+      <c r="Q17" s="11" t="n">
+        <f aca="false">R18-R15</f>
+        <v>0</v>
+      </c>
+      <c r="R17" s="11" t="n">
+        <f aca="false">U15-R15</f>
+        <v>0</v>
+      </c>
       <c r="U17" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="V17" s="11"/>
-      <c r="W17" s="11"/>
+      <c r="V17" s="11" t="n">
+        <f aca="false">W18-W15</f>
+        <v>0</v>
+      </c>
+      <c r="W17" s="11" t="n">
+        <f aca="false">Z15-W15</f>
+        <v>0</v>
+      </c>
       <c r="Z17" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="AA17" s="11"/>
+      <c r="AA17" s="11" t="n">
+        <f aca="false">AB18-AB15</f>
+        <v>0</v>
+      </c>
       <c r="AB17" s="11"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="n">
+        <f aca="false">C18-A17</f>
         <v>0</v>
       </c>
       <c r="B18" s="13"/>
-      <c r="C18" s="14"/>
-      <c r="F18" s="12"/>
+      <c r="C18" s="14" t="n">
+        <f aca="false">MIN(F18,F23)</f>
+        <v>2</v>
+      </c>
+      <c r="F18" s="12" t="n">
+        <f aca="false">H18-F17</f>
+        <v>2</v>
+      </c>
       <c r="G18" s="13"/>
-      <c r="H18" s="14"/>
-      <c r="K18" s="12"/>
+      <c r="H18" s="14" t="n">
+        <f aca="false">K18</f>
+        <v>10</v>
+      </c>
+      <c r="K18" s="12" t="n">
+        <f aca="false">M18-K17</f>
+        <v>10</v>
+      </c>
       <c r="L18" s="13"/>
-      <c r="M18" s="14"/>
-      <c r="P18" s="12"/>
+      <c r="M18" s="14" t="n">
+        <f aca="false">P18</f>
+        <v>16</v>
+      </c>
+      <c r="P18" s="12" t="n">
+        <f aca="false">R18-P17</f>
+        <v>16</v>
+      </c>
       <c r="Q18" s="13"/>
-      <c r="R18" s="14"/>
-      <c r="U18" s="12"/>
+      <c r="R18" s="14" t="n">
+        <f aca="false">U18</f>
+        <v>21</v>
+      </c>
+      <c r="U18" s="12" t="n">
+        <f aca="false">W18-U17</f>
+        <v>21</v>
+      </c>
       <c r="V18" s="13"/>
-      <c r="W18" s="14"/>
-      <c r="Z18" s="12"/>
+      <c r="W18" s="14" t="n">
+        <f aca="false">Z18</f>
+        <v>29</v>
+      </c>
+      <c r="Z18" s="12" t="n">
+        <f aca="false">AB18-Z17</f>
+        <v>29</v>
+      </c>
       <c r="AA18" s="13"/>
-      <c r="AB18" s="14"/>
+      <c r="AB18" s="14" t="n">
+        <f aca="false">AB15</f>
+        <v>33</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F20" s="6"/>
+      <c r="F20" s="6" t="n">
+        <f aca="false">C15</f>
+        <v>2</v>
+      </c>
       <c r="G20" s="7"/>
-      <c r="H20" s="8"/>
-      <c r="K20" s="6"/>
+      <c r="H20" s="8" t="n">
+        <f aca="false">F20+F22</f>
+        <v>10</v>
+      </c>
+      <c r="K20" s="6" t="n">
+        <f aca="false">H20</f>
+        <v>10</v>
+      </c>
       <c r="L20" s="7"/>
-      <c r="M20" s="8"/>
-      <c r="P20" s="6"/>
+      <c r="M20" s="8" t="n">
+        <f aca="false">K20+K22</f>
+        <v>18</v>
+      </c>
+      <c r="P20" s="6" t="n">
+        <f aca="false">M20</f>
+        <v>18</v>
+      </c>
       <c r="Q20" s="7"/>
-      <c r="R20" s="8"/>
-      <c r="U20" s="6"/>
+      <c r="R20" s="8" t="n">
+        <f aca="false">P20+P22</f>
+        <v>24</v>
+      </c>
+      <c r="U20" s="6" t="n">
+        <f aca="false">MAX(R20,R25)</f>
+        <v>24</v>
+      </c>
       <c r="V20" s="7"/>
-      <c r="W20" s="8"/>
+      <c r="W20" s="8" t="n">
+        <f aca="false">U20+U22</f>
+        <v>26</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F21" s="9" t="s">
@@ -1633,45 +2660,105 @@
       <c r="F22" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
+      <c r="G22" s="11" t="n">
+        <f aca="false">H23-H20</f>
+        <v>3</v>
+      </c>
+      <c r="H22" s="11" t="n">
+        <f aca="false">MIN(K20,K25)-H20</f>
+        <v>0</v>
+      </c>
       <c r="K22" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
+      <c r="L22" s="11" t="n">
+        <f aca="false">M23-M20</f>
+        <v>3</v>
+      </c>
+      <c r="M22" s="11" t="n">
+        <f aca="false">P20-M20</f>
+        <v>0</v>
+      </c>
       <c r="P22" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="11"/>
+      <c r="Q22" s="11" t="n">
+        <f aca="false">R23-R20</f>
+        <v>3</v>
+      </c>
+      <c r="R22" s="11" t="n">
+        <f aca="false">U20-R20</f>
+        <v>0</v>
+      </c>
       <c r="U22" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="V22" s="11"/>
-      <c r="W22" s="11"/>
+      <c r="V22" s="11" t="n">
+        <f aca="false">W23-W20</f>
+        <v>3</v>
+      </c>
+      <c r="W22" s="11" t="n">
+        <f aca="false">Z15-W20</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F23" s="12"/>
+      <c r="F23" s="12" t="n">
+        <f aca="false">H23-F22</f>
+        <v>5</v>
+      </c>
       <c r="G23" s="13"/>
-      <c r="H23" s="14"/>
-      <c r="K23" s="12"/>
+      <c r="H23" s="14" t="n">
+        <f aca="false">MIN(K23,K28)</f>
+        <v>13</v>
+      </c>
+      <c r="K23" s="12" t="n">
+        <f aca="false">M23-K22</f>
+        <v>13</v>
+      </c>
       <c r="L23" s="13"/>
-      <c r="M23" s="14"/>
-      <c r="P23" s="12"/>
+      <c r="M23" s="14" t="n">
+        <f aca="false">P23</f>
+        <v>21</v>
+      </c>
+      <c r="P23" s="12" t="n">
+        <f aca="false">R23-P22</f>
+        <v>21</v>
+      </c>
       <c r="Q23" s="13"/>
-      <c r="R23" s="14"/>
-      <c r="U23" s="12"/>
+      <c r="R23" s="14" t="n">
+        <f aca="false">U23</f>
+        <v>27</v>
+      </c>
+      <c r="U23" s="12" t="n">
+        <f aca="false">W23-U22</f>
+        <v>27</v>
+      </c>
       <c r="V23" s="13"/>
-      <c r="W23" s="14"/>
+      <c r="W23" s="14" t="n">
+        <f aca="false">Z18</f>
+        <v>29</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K25" s="6"/>
+      <c r="K25" s="6" t="n">
+        <f aca="false">H20</f>
+        <v>10</v>
+      </c>
       <c r="L25" s="7"/>
-      <c r="M25" s="8"/>
-      <c r="P25" s="6"/>
+      <c r="M25" s="8" t="n">
+        <f aca="false">K25+K27</f>
+        <v>18</v>
+      </c>
+      <c r="P25" s="6" t="n">
+        <f aca="false">M25</f>
+        <v>18</v>
+      </c>
       <c r="Q25" s="7"/>
-      <c r="R25" s="8"/>
+      <c r="R25" s="8" t="n">
+        <f aca="false">P25+P27</f>
+        <v>23</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K26" s="9" t="s">
@@ -1689,21 +2776,45 @@
       <c r="K27" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
+      <c r="L27" s="11" t="n">
+        <f aca="false">M28-M25</f>
+        <v>4</v>
+      </c>
+      <c r="M27" s="11" t="n">
+        <f aca="false">P25-M25</f>
+        <v>0</v>
+      </c>
       <c r="P27" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="11"/>
+      <c r="Q27" s="11" t="n">
+        <f aca="false">R28-R25</f>
+        <v>4</v>
+      </c>
+      <c r="R27" s="11" t="n">
+        <f aca="false">U20-R25</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K28" s="12"/>
+      <c r="K28" s="12" t="n">
+        <f aca="false">M28-K27</f>
+        <v>14</v>
+      </c>
       <c r="L28" s="13"/>
-      <c r="M28" s="14"/>
-      <c r="P28" s="12"/>
+      <c r="M28" s="14" t="n">
+        <f aca="false">P28</f>
+        <v>22</v>
+      </c>
+      <c r="P28" s="12" t="n">
+        <f aca="false">R28-P27</f>
+        <v>22</v>
+      </c>
       <c r="Q28" s="13"/>
-      <c r="R28" s="14"/>
+      <c r="R28" s="14" t="n">
+        <f aca="false">U23</f>
+        <v>27</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="15"/>
@@ -1982,6 +3093,11 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B17 G17 G22 L17 L22 L27 Q17 Q22 Q27 V17 V22 AA17">
+    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1998,13 +3114,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="3.83"/>
   </cols>
@@ -2098,7 +3214,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="2" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2134,7 +3250,7 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="2" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2166,7 +3282,9 @@
       <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="D9" s="5"/>
       <c r="E9" s="4" t="s">
         <v>11</v>
@@ -2234,7 +3352,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2263,7 +3381,53 @@
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="8" t="n">
-        <v>0</v>
+        <f aca="false">A15+A17</f>
+        <v>6</v>
+      </c>
+      <c r="F15" s="6" t="n">
+        <f aca="false">C15</f>
+        <v>6</v>
+      </c>
+      <c r="G15" s="7"/>
+      <c r="H15" s="8" t="n">
+        <f aca="false">F15+F17</f>
+        <v>13</v>
+      </c>
+      <c r="K15" s="6" t="n">
+        <f aca="false">H15</f>
+        <v>13</v>
+      </c>
+      <c r="L15" s="7"/>
+      <c r="M15" s="8" t="n">
+        <f aca="false">K15+K17</f>
+        <v>17</v>
+      </c>
+      <c r="P15" s="6" t="n">
+        <f aca="false">M15</f>
+        <v>17</v>
+      </c>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="8" t="n">
+        <f aca="false">P15+P17</f>
+        <v>20</v>
+      </c>
+      <c r="U15" s="6" t="n">
+        <f aca="false">MAX(R15,R21)</f>
+        <v>24</v>
+      </c>
+      <c r="V15" s="7"/>
+      <c r="W15" s="8" t="n">
+        <f aca="false">U15+U17</f>
+        <v>32</v>
+      </c>
+      <c r="Z15" s="6" t="n">
+        <f aca="false">MAX(W15,W21,W27)</f>
+        <v>33</v>
+      </c>
+      <c r="AA15" s="7"/>
+      <c r="AB15" s="8" t="n">
+        <f aca="false">Z15+Z17</f>
+        <v>41</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2272,6 +3436,31 @@
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
+      <c r="F16" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="K16" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="P16" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="U16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="Z16" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA16" s="9"/>
+      <c r="AB16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="n">
@@ -2279,30 +3468,382 @@
         <v>6</v>
       </c>
       <c r="B17" s="11" t="n">
+        <f aca="false">C18-C15</f>
         <v>0</v>
       </c>
       <c r="C17" s="11" t="n">
+        <f aca="false">MIN(F15,F21)-C15</f>
         <v>0</v>
       </c>
+      <c r="F17" s="10" t="n">
+        <f aca="false">H3</f>
+        <v>7</v>
+      </c>
+      <c r="G17" s="11" t="n">
+        <f aca="false">H18-H15</f>
+        <v>5</v>
+      </c>
+      <c r="H17" s="11" t="n">
+        <f aca="false">K15-H15</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="10" t="n">
+        <f aca="false">H5</f>
+        <v>4</v>
+      </c>
+      <c r="L17" s="11" t="n">
+        <f aca="false">M18-M15</f>
+        <v>5</v>
+      </c>
+      <c r="M17" s="11" t="n">
+        <f aca="false">P15-M15</f>
+        <v>0</v>
+      </c>
+      <c r="P17" s="10" t="n">
+        <f aca="false">H8</f>
+        <v>3</v>
+      </c>
+      <c r="Q17" s="11" t="n">
+        <f aca="false">R18-R15</f>
+        <v>5</v>
+      </c>
+      <c r="R17" s="11" t="n">
+        <f aca="false">U15-R15</f>
+        <v>4</v>
+      </c>
+      <c r="U17" s="10" t="n">
+        <f aca="false">H11</f>
+        <v>8</v>
+      </c>
+      <c r="V17" s="11" t="n">
+        <f aca="false">W18-W15</f>
+        <v>1</v>
+      </c>
+      <c r="W17" s="11" t="n">
+        <f aca="false">Z15-W15</f>
+        <v>1</v>
+      </c>
+      <c r="Z17" s="10" t="n">
+        <f aca="false">H13</f>
+        <v>8</v>
+      </c>
+      <c r="AA17" s="11" t="n">
+        <f aca="false">AB18-AB15</f>
+        <v>0</v>
+      </c>
+      <c r="AB17" s="11"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="n">
+        <f aca="false">C18-A17</f>
         <v>0</v>
       </c>
       <c r="B18" s="13"/>
       <c r="C18" s="14" t="n">
         <f aca="false">MIN(F18,F24)</f>
+        <v>6</v>
+      </c>
+      <c r="F18" s="12" t="n">
+        <f aca="false">H18-F17</f>
+        <v>11</v>
+      </c>
+      <c r="G18" s="13"/>
+      <c r="H18" s="14" t="n">
+        <f aca="false">K18</f>
+        <v>18</v>
+      </c>
+      <c r="K18" s="12" t="n">
+        <f aca="false">M18-K17</f>
+        <v>18</v>
+      </c>
+      <c r="L18" s="13"/>
+      <c r="M18" s="14" t="n">
+        <f aca="false">P18</f>
+        <v>22</v>
+      </c>
+      <c r="P18" s="12" t="n">
+        <f aca="false">R18-P17</f>
+        <v>22</v>
+      </c>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="14" t="n">
+        <f aca="false">U18</f>
+        <v>25</v>
+      </c>
+      <c r="U18" s="12" t="n">
+        <f aca="false">W18-U17</f>
+        <v>25</v>
+      </c>
+      <c r="V18" s="13"/>
+      <c r="W18" s="14" t="n">
+        <f aca="false">Z18</f>
+        <v>33</v>
+      </c>
+      <c r="Z18" s="12" t="n">
+        <f aca="false">AB18-Z17</f>
+        <v>33</v>
+      </c>
+      <c r="AA18" s="13"/>
+      <c r="AB18" s="14" t="n">
+        <f aca="false">AB15</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F21" s="6" t="n">
+        <f aca="false">C15</f>
+        <v>6</v>
+      </c>
+      <c r="G21" s="7"/>
+      <c r="H21" s="8" t="n">
+        <f aca="false">F21+F23</f>
+        <v>13</v>
+      </c>
+      <c r="K21" s="6" t="n">
+        <f aca="false">H21</f>
+        <v>13</v>
+      </c>
+      <c r="L21" s="7"/>
+      <c r="M21" s="8" t="n">
+        <f aca="false">K21+K23</f>
+        <v>17</v>
+      </c>
+      <c r="P21" s="6" t="n">
+        <f aca="false">MAX(M21,M27)</f>
+        <v>18</v>
+      </c>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="8" t="n">
+        <f aca="false">P21+P23</f>
+        <v>24</v>
+      </c>
+      <c r="U21" s="6" t="n">
+        <f aca="false">R21</f>
+        <v>24</v>
+      </c>
+      <c r="V21" s="7"/>
+      <c r="W21" s="8" t="n">
+        <f aca="false">U21+U23</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F22" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="K22" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="P22" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="U22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="V22" s="9"/>
+      <c r="W22" s="9"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F23" s="10" t="n">
+        <f aca="false">H4</f>
+        <v>7</v>
+      </c>
+      <c r="G23" s="11" t="n">
+        <f aca="false">H24-H21</f>
         <v>0</v>
       </c>
+      <c r="H23" s="11" t="n">
+        <f aca="false">MIN(K21,K27)-H21</f>
+        <v>0</v>
+      </c>
+      <c r="K23" s="10" t="n">
+        <f aca="false">H6</f>
+        <v>4</v>
+      </c>
+      <c r="L23" s="11" t="n">
+        <f aca="false">M24-M21</f>
+        <v>1</v>
+      </c>
+      <c r="M23" s="11" t="n">
+        <f aca="false">P21-M21</f>
+        <v>1</v>
+      </c>
+      <c r="P23" s="10" t="n">
+        <f aca="false">H9</f>
+        <v>6</v>
+      </c>
+      <c r="Q23" s="11" t="n">
+        <f aca="false">R24-R21</f>
+        <v>0</v>
+      </c>
+      <c r="R23" s="11" t="n">
+        <f aca="false">MIN(U15,U21,U27)-R21</f>
+        <v>0</v>
+      </c>
+      <c r="U23" s="10" t="n">
+        <f aca="false">H10</f>
+        <v>2</v>
+      </c>
+      <c r="V23" s="11" t="n">
+        <f aca="false">W24-W21</f>
+        <v>7</v>
+      </c>
+      <c r="W23" s="11" t="n">
+        <f aca="false">Z15-W21</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F24" s="12" t="n">
+        <f aca="false">H24-F23</f>
+        <v>6</v>
+      </c>
+      <c r="G24" s="13"/>
+      <c r="H24" s="14" t="n">
+        <f aca="false">MIN(K24,K30)</f>
+        <v>13</v>
+      </c>
+      <c r="K24" s="12" t="n">
+        <f aca="false">M24-K23</f>
+        <v>14</v>
+      </c>
+      <c r="L24" s="13"/>
+      <c r="M24" s="14" t="n">
+        <f aca="false">P24</f>
+        <v>18</v>
+      </c>
+      <c r="P24" s="12" t="n">
+        <f aca="false">R24-P23</f>
+        <v>18</v>
+      </c>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="14" t="n">
+        <f aca="false">MIN(U18,U24,U30)</f>
+        <v>24</v>
+      </c>
+      <c r="U24" s="12" t="n">
+        <f aca="false">W24-U23</f>
+        <v>31</v>
+      </c>
+      <c r="V24" s="13"/>
+      <c r="W24" s="14" t="n">
+        <f aca="false">Z18</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K27" s="6" t="n">
+        <f aca="false">H21</f>
+        <v>13</v>
+      </c>
+      <c r="L27" s="7"/>
+      <c r="M27" s="8" t="n">
+        <f aca="false">K27+K29</f>
+        <v>18</v>
+      </c>
+      <c r="U27" s="6" t="n">
+        <f aca="false">R21</f>
+        <v>24</v>
+      </c>
+      <c r="V27" s="7"/>
+      <c r="W27" s="8" t="n">
+        <f aca="false">U27+U29</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K28" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="U28" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K29" s="10" t="n">
+        <f aca="false">H7</f>
+        <v>5</v>
+      </c>
+      <c r="L29" s="11" t="n">
+        <f aca="false">M30-M27</f>
+        <v>0</v>
+      </c>
+      <c r="M29" s="11" t="n">
+        <f aca="false">P21-M27</f>
+        <v>0</v>
+      </c>
+      <c r="U29" s="10" t="n">
+        <f aca="false">H12</f>
+        <v>9</v>
+      </c>
+      <c r="V29" s="11" t="n">
+        <f aca="false">W30-W27</f>
+        <v>0</v>
+      </c>
+      <c r="W29" s="11" t="n">
+        <f aca="false">Z15-W27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K30" s="12" t="n">
+        <f aca="false">M30-K29</f>
+        <v>13</v>
+      </c>
+      <c r="L30" s="13"/>
+      <c r="M30" s="14" t="n">
+        <f aca="false">P24</f>
+        <v>18</v>
+      </c>
+      <c r="U30" s="12" t="n">
+        <f aca="false">W30-U29</f>
+        <v>24</v>
+      </c>
+      <c r="V30" s="13"/>
+      <c r="W30" s="14" t="n">
+        <f aca="false">Z18</f>
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="14">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="A16:C16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="U16:W16"/>
+    <mergeCell ref="Z16:AB16"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="P22:R22"/>
+    <mergeCell ref="U22:W22"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="U28:W28"/>
   </mergeCells>
-  <conditionalFormatting sqref="B16">
+  <conditionalFormatting sqref="B16 G16 G22 L16 L22 L28 Q16 Q22 V16 V22 V28 AA16">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17 G17 G23 H8 L17 L29 Q17 Q23 V17 V29 AA17">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17 G17 G23 L17 L23 L29 Q17 Q23 V17 V23 V29 AA17">
+    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2313,5 +3854,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CSeite &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>